<commit_message>
Finalizing data preparation national data
- data preparation national data finalized
- generating new file for data preparation regional data
</commit_message>
<xml_diff>
--- a/Bevölkerungsentwicklung_Schweiz_2000-2020.xlsx
+++ b/Bevölkerungsentwicklung_Schweiz_2000-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabie\Universität St.Gallen\Software-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA3B218-4237-43C9-B2A1-A4EFC27EA09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAF727A-64D1-4841-A6EF-06C1F01F2028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="35" r:id="rId1"/>
@@ -953,6 +953,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -974,8 +976,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1326,16 +1326,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="71" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1343,187 +1343,187 @@
       <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" s="79">
-        <f>'2010'!B6</f>
-        <v>7870134</v>
-      </c>
-      <c r="C2" s="79">
-        <f>'2010'!H6</f>
-        <v>6103857</v>
-      </c>
-      <c r="D2" s="79">
-        <f>'2010'!I6</f>
-        <v>1766277</v>
+      <c r="B2" s="72">
+        <f>'2010'!B6/1000</f>
+        <v>7870.134</v>
+      </c>
+      <c r="C2" s="72">
+        <f>'2010'!H6/1000</f>
+        <v>6103.857</v>
+      </c>
+      <c r="D2" s="72">
+        <f>'2010'!I6/1000</f>
+        <v>1766.277</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" s="79">
-        <f>'2011'!B6</f>
-        <v>7954662</v>
-      </c>
-      <c r="C3" s="79">
-        <f>'2011'!H6</f>
-        <v>6138668</v>
-      </c>
-      <c r="D3" s="79">
-        <f>'2011'!I6</f>
-        <v>1815994</v>
+      <c r="B3" s="72">
+        <f>'2011'!B6/1000</f>
+        <v>7954.6620000000003</v>
+      </c>
+      <c r="C3" s="72">
+        <f>'2011'!H6/1000</f>
+        <v>6138.6679999999997</v>
+      </c>
+      <c r="D3" s="72">
+        <f>'2011'!I6/1000</f>
+        <v>1815.9939999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
-      <c r="B4" s="79">
-        <f>'2012'!B6</f>
-        <v>8039060</v>
-      </c>
-      <c r="C4" s="79">
-        <f>'2012'!H6</f>
-        <v>6169091</v>
-      </c>
-      <c r="D4" s="79">
-        <f>'2012'!I6</f>
-        <v>1869969</v>
+      <c r="B4" s="72">
+        <f>'2012'!B6/1000</f>
+        <v>8039.06</v>
+      </c>
+      <c r="C4" s="72">
+        <f>'2012'!H6/1000</f>
+        <v>6169.0910000000003</v>
+      </c>
+      <c r="D4" s="72">
+        <f>'2012'!I6/1000</f>
+        <v>1869.9690000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
-      <c r="B5" s="79">
-        <f>'2013'!B6</f>
-        <v>8139631</v>
-      </c>
-      <c r="C5" s="79">
-        <f>'2013'!H6</f>
-        <v>6202184</v>
-      </c>
-      <c r="D5" s="79">
-        <f>'2013'!I6</f>
-        <v>1937447</v>
+      <c r="B5" s="72">
+        <f>'2013'!B6/1000</f>
+        <v>8139.6310000000003</v>
+      </c>
+      <c r="C5" s="72">
+        <f>'2013'!H6/1000</f>
+        <v>6202.1840000000002</v>
+      </c>
+      <c r="D5" s="72">
+        <f>'2013'!I6/1000</f>
+        <v>1937.4469999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" s="79">
-        <f>'2014'!B6</f>
-        <v>8237666</v>
-      </c>
-      <c r="C6" s="79">
-        <f>'2014'!H6</f>
-        <v>6239207</v>
-      </c>
-      <c r="D6" s="79">
-        <f>'2014'!I6</f>
-        <v>1998459</v>
+      <c r="B6" s="72">
+        <f>'2014'!B6/1000</f>
+        <v>8237.6659999999993</v>
+      </c>
+      <c r="C6" s="72">
+        <f>'2014'!H6/1000</f>
+        <v>6239.2070000000003</v>
+      </c>
+      <c r="D6" s="72">
+        <f>'2014'!I6/1000</f>
+        <v>1998.4590000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" s="79">
-        <f>'2015'!B6</f>
-        <v>8327126</v>
-      </c>
-      <c r="C7" s="79">
-        <f>'2015'!H6</f>
-        <v>6278459</v>
-      </c>
-      <c r="D7" s="79">
-        <f>'2015'!I6</f>
-        <v>2048667</v>
+      <c r="B7" s="72">
+        <f>'2015'!B6/1000</f>
+        <v>8327.1260000000002</v>
+      </c>
+      <c r="C7" s="72">
+        <f>'2015'!H6/1000</f>
+        <v>6278.4589999999998</v>
+      </c>
+      <c r="D7" s="72">
+        <f>'2015'!I6/1000</f>
+        <v>2048.6669999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
-      <c r="B8" s="79">
-        <f>'2016'!B6</f>
-        <v>8419550</v>
-      </c>
-      <c r="C8" s="79">
-        <f>'2016'!H6</f>
-        <v>6318404</v>
-      </c>
-      <c r="D8" s="79">
-        <f>'2016'!I6</f>
-        <v>2101146</v>
+      <c r="B8" s="72">
+        <f>'2016'!B6/1000</f>
+        <v>8419.5499999999993</v>
+      </c>
+      <c r="C8" s="72">
+        <f>'2016'!H6/1000</f>
+        <v>6318.4040000000005</v>
+      </c>
+      <c r="D8" s="72">
+        <f>'2016'!I6/1000</f>
+        <v>2101.1460000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
-      <c r="B9" s="79">
-        <f>'2017'!B6</f>
-        <v>8484130</v>
-      </c>
-      <c r="C9" s="79">
-        <f>'2017'!H6</f>
-        <v>6357738</v>
-      </c>
-      <c r="D9" s="79">
-        <f>'2017'!I6</f>
-        <v>2126392</v>
+      <c r="B9" s="72">
+        <f>'2017'!B6/1000</f>
+        <v>8484.1299999999992</v>
+      </c>
+      <c r="C9" s="72">
+        <f>'2017'!H6/1000</f>
+        <v>6357.7380000000003</v>
+      </c>
+      <c r="D9" s="72">
+        <f>'2017'!I6/1000</f>
+        <v>2126.3919999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
-      <c r="B10" s="79">
-        <f>'2018'!B6</f>
-        <v>8544527</v>
-      </c>
-      <c r="C10" s="79">
-        <f>'2018'!H6</f>
-        <v>6396252</v>
-      </c>
-      <c r="D10" s="79">
-        <f>'2018'!I6</f>
-        <v>2148275</v>
+      <c r="B10" s="72">
+        <f>'2018'!B6/1000</f>
+        <v>8544.527</v>
+      </c>
+      <c r="C10" s="72">
+        <f>'2018'!H6/1000</f>
+        <v>6396.2520000000004</v>
+      </c>
+      <c r="D10" s="72">
+        <f>'2018'!I6/1000</f>
+        <v>2148.2750000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
-      <c r="B11" s="79">
-        <f>'2019'!B6</f>
-        <v>8606033</v>
-      </c>
-      <c r="C11" s="79">
-        <f>'2019'!H6</f>
-        <v>6430658</v>
-      </c>
-      <c r="D11" s="79">
-        <f>'2019'!I6</f>
-        <v>2175375</v>
+      <c r="B11" s="72">
+        <f>'2019'!B6/1000</f>
+        <v>8606.0329999999994</v>
+      </c>
+      <c r="C11" s="72">
+        <f>'2019'!H6/1000</f>
+        <v>6430.6580000000004</v>
+      </c>
+      <c r="D11" s="72">
+        <f>'2019'!I6/1000</f>
+        <v>2175.375</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" s="79">
-        <f>'2020'!B6</f>
-        <v>8670300</v>
-      </c>
-      <c r="C12" s="79">
-        <f>'2020'!H6</f>
-        <v>6459512</v>
-      </c>
-      <c r="D12" s="79">
-        <f>'2020'!I6</f>
-        <v>2210788</v>
+      <c r="B12" s="72">
+        <f>'2020'!B6/1000</f>
+        <v>8670.2999999999993</v>
+      </c>
+      <c r="C12" s="72">
+        <f>'2020'!H6/1000</f>
+        <v>6459.5119999999997</v>
+      </c>
+      <c r="D12" s="72">
+        <f>'2020'!I6/1000</f>
+        <v>2210.788</v>
       </c>
     </row>
   </sheetData>
@@ -1663,10 +1663,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -1693,8 +1693,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -1719,8 +1719,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -3823,10 +3823,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -3853,8 +3853,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -3879,8 +3879,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -5983,10 +5983,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -6013,8 +6013,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -6039,8 +6039,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -8133,10 +8133,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -8155,8 +8155,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
@@ -8170,8 +8170,8 @@
       <c r="I5" s="41"/>
       <c r="J5" s="41"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
@@ -8184,8 +8184,8 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -9667,10 +9667,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9689,8 +9689,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -9703,8 +9703,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -9718,8 +9718,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -11201,10 +11201,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -11223,8 +11223,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -11237,8 +11237,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -11252,8 +11252,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -12735,10 +12735,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -12757,8 +12757,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -12771,8 +12771,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -12786,8 +12786,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -14269,10 +14269,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -14291,8 +14291,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -14305,8 +14305,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -14320,8 +14320,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -15803,10 +15803,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -15825,8 +15825,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -15839,8 +15839,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -15854,8 +15854,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -17344,10 +17344,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -17366,8 +17366,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -17380,8 +17380,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -17395,8 +17395,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -18912,10 +18912,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -18942,8 +18942,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -18968,8 +18968,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -21050,10 +21050,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -21072,8 +21072,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -21086,8 +21086,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -21101,8 +21101,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -22583,10 +22583,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -22605,8 +22605,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -22619,8 +22619,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -22634,8 +22634,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -24116,10 +24116,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -24138,8 +24138,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -24152,8 +24152,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -24167,8 +24167,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -25649,10 +25649,10 @@
       <c r="K3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="75" t="s">
+      <c r="M3" s="77" t="s">
         <v>99</v>
       </c>
     </row>
@@ -25671,8 +25671,8 @@
       <c r="K4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="76"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
@@ -25685,8 +25685,8 @@
       <c r="I5" s="43"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="76"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
@@ -25700,8 +25700,8 @@
       <c r="I6" s="44"/>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" s="36" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -27217,10 +27217,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -27247,8 +27247,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -27273,8 +27273,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -29391,10 +29391,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -29421,8 +29421,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -29447,8 +29447,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -31564,10 +31564,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -31594,8 +31594,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -31620,8 +31620,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -33736,10 +33736,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -33766,8 +33766,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -33792,8 +33792,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -35908,10 +35908,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -35938,8 +35938,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -35964,8 +35964,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -38080,10 +38080,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -38110,8 +38110,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -38136,8 +38136,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">
@@ -40252,10 +40252,10 @@
       <c r="N3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="73" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="39" t="s">
@@ -40282,8 +40282,8 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="39" t="s">
         <v>77</v>
       </c>
@@ -40308,8 +40308,8 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="76"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="64"/>
       <c r="S5" s="43" t="s">

</xml_diff>